<commit_message>
Unit tests to produce Performance comparable results
</commit_message>
<xml_diff>
--- a/VirtualObjects.Tests/Sessions/Performance.xlsx
+++ b/VirtualObjects.Tests/Sessions/Performance.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>VirtualObjects</t>
   </si>
@@ -36,7 +36,10 @@
     <t>Atempt</t>
   </si>
   <si>
-    <t>Diff</t>
+    <t>HardCoded</t>
+  </si>
+  <si>
+    <t>EntityFramework</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>CountSuppliers!$B$1</c:f>
+              <c:f>CountSuppliers!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -156,10 +159,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>CountSuppliers!$B$2:$B$50</c:f>
+              <c:f>CountSuppliers!$C$3:$C$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="48"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -170,7 +173,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>CountSuppliers!$C$1</c:f>
+              <c:f>CountSuppliers!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -199,10 +202,53 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>CountSuppliers!$C$2:$C$50</c:f>
+              <c:f>CountSuppliers!$D$3:$D$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CountSuppliers!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HardCoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>CountSuppliers!$E$3:$E$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -210,14 +256,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>CountSuppliers!$D$1</c:f>
+              <c:f>CountSuppliers!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Diff</c:v>
+                  <c:v>EntityFramework</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -242,10 +288,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>CountSuppliers!$D$2:$D$50</c:f>
+              <c:f>CountSuppliers!$B$3:$B$50</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -260,11 +306,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="228798592"/>
-        <c:axId val="228800552"/>
+        <c:axId val="291155616"/>
+        <c:axId val="291156400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="228798592"/>
+        <c:axId val="291155616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,7 +351,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228800552"/>
+        <c:crossAx val="291156400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -313,7 +359,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228800552"/>
+        <c:axId val="291156400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -363,7 +409,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228798592"/>
+        <c:crossAx val="291155616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -994,13 +1040,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
@@ -1319,44 +1365,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="16.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
-        <f>SUM(B2:B96)</f>
-        <v>0</v>
-      </c>
-      <c r="G1" s="2">
-        <f>SUM(C2:C96)</f>
-        <v>0</v>
-      </c>
-      <c r="H1" s="2">
-        <f>SUM(D2:D96)</f>
-        <v>0</v>
-      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EF is quite fast this days...
</commit_message>
<xml_diff>
--- a/VirtualObjects.Tests/Sessions/Performance.xlsx
+++ b/VirtualObjects.Tests/Sessions/Performance.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="PerfRecord" sheetId="2" r:id="rId1"/>
-    <sheet name="CountSuppliers" sheetId="3" r:id="rId2"/>
+    <sheet name="MappingSuppliers" sheetId="4" r:id="rId2"/>
+    <sheet name="CountSuppliers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>VirtualObjects</t>
   </si>
@@ -106,6 +107,401 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingSuppliers!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VirtualObjects</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingSuppliers!$C$3:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingSuppliers!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dapper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingSuppliers!$D$3:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingSuppliers!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HardCoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingSuppliers!$E$3:$E$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingSuppliers!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EntityFramework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingSuppliers!$B$3:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="296557312"/>
+        <c:axId val="296553392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="296557312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296553392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="296553392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296557312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-PT"/>
@@ -306,11 +702,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="291155616"/>
-        <c:axId val="291156400"/>
+        <c:axId val="229533360"/>
+        <c:axId val="229526696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="291155616"/>
+        <c:axId val="229533360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -351,7 +747,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291156400"/>
+        <c:crossAx val="229526696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -359,7 +755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291156400"/>
+        <c:axId val="229526696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -409,7 +805,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291155616"/>
+        <c:crossAx val="229533360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -540,6 +936,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -1036,7 +1472,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1403,4 +2372,46 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Creating a proxy via code Generation
</commit_message>
<xml_diff>
--- a/VirtualObjects.Tests/Sessions/Performance.xlsx
+++ b/VirtualObjects.Tests/Sessions/Performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MappingSuppliers" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>VirtualObjects</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Compiled</t>
+  </si>
+  <si>
+    <t>EntityProxyProvider</t>
   </si>
 </sst>
 </file>
@@ -370,11 +373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="303810544"/>
-        <c:axId val="303810936"/>
+        <c:axId val="309812752"/>
+        <c:axId val="309814320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="303810544"/>
+        <c:axId val="309812752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +419,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303810936"/>
+        <c:crossAx val="309814320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -424,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303810936"/>
+        <c:axId val="309814320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +477,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303810544"/>
+        <c:crossAx val="309812752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -801,11 +804,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="303807016"/>
-        <c:axId val="303808584"/>
+        <c:axId val="309811576"/>
+        <c:axId val="309808832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="303807016"/>
+        <c:axId val="309811576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +850,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303808584"/>
+        <c:crossAx val="309808832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -855,7 +858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303808584"/>
+        <c:axId val="309808832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +908,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303807016"/>
+        <c:crossAx val="309811576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1020,7 +1023,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>EntitiesCreation!$C$1</c:f>
+              <c:f>EntitiesCreation!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1058,7 +1061,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EntitiesCreation!$C$3:$C$50</c:f>
+              <c:f>EntitiesCreation!$D$3:$D$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="48"/>
@@ -1072,7 +1075,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>EntitiesCreation!$D$1</c:f>
+              <c:f>EntitiesCreation!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1110,7 +1113,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EntitiesCreation!$D$3:$D$50</c:f>
+              <c:f>EntitiesCreation!$E$3:$E$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="48"/>
@@ -1124,7 +1127,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>EntitiesCreation!$E$1</c:f>
+              <c:f>EntitiesCreation!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1162,7 +1165,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EntitiesCreation!$E$3:$E$50</c:f>
+              <c:f>EntitiesCreation!$F$3:$F$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="48"/>
@@ -1223,6 +1226,49 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesCreation!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EntityProxyProvider</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesCreation!$C$3:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1232,11 +1278,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="303807800"/>
-        <c:axId val="240102944"/>
+        <c:axId val="310204136"/>
+        <c:axId val="310204920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="303807800"/>
+        <c:axId val="310204136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1324,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240102944"/>
+        <c:crossAx val="310204920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1286,7 +1332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240102944"/>
+        <c:axId val="310204920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1382,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303807800"/>
+        <c:crossAx val="310204136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1716,11 +1762,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="303163808"/>
-        <c:axId val="303163416"/>
+        <c:axId val="310203352"/>
+        <c:axId val="310692736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="303163808"/>
+        <c:axId val="310203352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1808,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303163416"/>
+        <c:crossAx val="310692736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1770,7 +1816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303163416"/>
+        <c:axId val="310692736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1866,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303163808"/>
+        <c:crossAx val="310203352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4131,13 +4177,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -4546,20 +4592,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -4567,17 +4613,20 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4589,7 +4638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added performance check test for Order details.
</commit_message>
<xml_diff>
--- a/VirtualObjects.Tests/Sessions/Performance.xlsx
+++ b/VirtualObjects.Tests/Sessions/Performance.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
-    <sheet name="MappingSuppliers" sheetId="4" r:id="rId1"/>
-    <sheet name="CountSuppliers" sheetId="3" r:id="rId2"/>
-    <sheet name="EntitiesCreation" sheetId="5" r:id="rId3"/>
-    <sheet name="EntitiesMapping" sheetId="6" r:id="rId4"/>
+    <sheet name="MappingOrderDetails" sheetId="7" r:id="rId1"/>
+    <sheet name="MappingSuppliers" sheetId="4" r:id="rId2"/>
+    <sheet name="CountSuppliers" sheetId="3" r:id="rId3"/>
+    <sheet name="EntitiesCreation" sheetId="5" r:id="rId4"/>
+    <sheet name="EntitiesMapping" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>VirtualObjects</t>
   </si>
@@ -137,6 +138,556 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingOrderDetails!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VirtualObjects</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$C$3:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingOrderDetails!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dapper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$D$3:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingOrderDetails!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HardCoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$E$3:$E$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingOrderDetails!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EntityFramework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingOrderDetails!$B$3:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1710590496"/>
+        <c:axId val="-1710589408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1710590496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t> os executions</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1710589408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1710589408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t> in Milliseconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1710590496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -373,11 +924,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1691972976"/>
-        <c:axId val="1691976784"/>
+        <c:axId val="-1890209216"/>
+        <c:axId val="-1890196160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1691972976"/>
+        <c:axId val="-1890209216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,7 +1029,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691976784"/>
+        <c:crossAx val="-1890196160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -486,7 +1037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1691976784"/>
+        <c:axId val="-1890196160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +1146,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691972976"/>
+        <c:crossAx val="-1890209216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -686,7 +1237,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -923,11 +1474,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1691963184"/>
-        <c:axId val="1691963728"/>
+        <c:axId val="-1890201056"/>
+        <c:axId val="-1890206496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1691963184"/>
+        <c:axId val="-1890201056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1579,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691963728"/>
+        <c:crossAx val="-1890206496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1036,7 +1587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1691963728"/>
+        <c:axId val="-1890206496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,7 +1691,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691963184"/>
+        <c:crossAx val="-1890201056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1231,7 +1782,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1511,11 +2062,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1691965360"/>
-        <c:axId val="1691969712"/>
+        <c:axId val="-1890199424"/>
+        <c:axId val="-1890207584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1691965360"/>
+        <c:axId val="-1890199424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1557,7 +2108,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691969712"/>
+        <c:crossAx val="-1890207584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1565,7 +2116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1691969712"/>
+        <c:axId val="-1890207584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +2166,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691965360"/>
+        <c:crossAx val="-1890199424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1629,7 +2180,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1706,7 +2256,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1995,11 +2545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1691973520"/>
-        <c:axId val="1691974064"/>
+        <c:axId val="-1890205408"/>
+        <c:axId val="-1890203776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1691973520"/>
+        <c:axId val="-1890205408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2041,7 +2591,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691974064"/>
+        <c:crossAx val="-1890203776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2049,7 +2599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1691974064"/>
+        <c:axId val="-1890203776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2649,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1691973520"/>
+        <c:crossAx val="-1890205408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2113,7 +2663,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2350,6 +2899,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -3839,6 +4428,502 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4389,6 +5474,43 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4406,7 +5528,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4443,7 +5565,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4745,7 +5867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4785,7 +5907,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4823,7 +5985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -4867,7 +6029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Performance Analysis after changing the way dynamics are mapped
</commit_message>
<xml_diff>
--- a/VirtualObjects.Tests/Sessions/Performance.xlsx
+++ b/VirtualObjects.Tests/Sessions/Performance.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projectos\VirtualObjects\VirtualObjects.Tests\Sessions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projectos\VirtualObjects\VirtualObjects.Tests\Sessions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
-    <sheet name="MappingOrderDetails" sheetId="7" r:id="rId1"/>
-    <sheet name="MappingSuppliers" sheetId="4" r:id="rId2"/>
-    <sheet name="CountSuppliers" sheetId="3" r:id="rId3"/>
-    <sheet name="EntitiesCreation" sheetId="5" r:id="rId4"/>
-    <sheet name="EntitiesMapping" sheetId="6" r:id="rId5"/>
+    <sheet name="MappingDynamicSuppliers" sheetId="8" r:id="rId1"/>
+    <sheet name="MappingOrderDetails" sheetId="7" r:id="rId2"/>
+    <sheet name="MappingSuppliers" sheetId="4" r:id="rId3"/>
+    <sheet name="CountSuppliers" sheetId="3" r:id="rId4"/>
+    <sheet name="EntitiesCreation" sheetId="5" r:id="rId5"/>
+    <sheet name="EntitiesMapping" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>VirtualObjects</t>
   </si>
@@ -140,7 +141,557 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingDynamicSuppliers!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VirtualObjects</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$C$3:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingDynamicSuppliers!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dapper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$D$3:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingDynamicSuppliers!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HardCoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$E$3:$E$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MappingDynamicSuppliers!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EntityFramework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$A$3:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MappingDynamicSuppliers!$B$3:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="299255424"/>
+        <c:axId val="234290464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="299255424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t> oF executions</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="234290464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="234290464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t> in Milliseconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299255424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -374,11 +925,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1710590496"/>
-        <c:axId val="-1710589408"/>
+        <c:axId val="298921416"/>
+        <c:axId val="298922984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1710590496"/>
+        <c:axId val="298921416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +959,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="pt-PT" baseline="0"/>
-                  <a:t> os executions</a:t>
+                  <a:t> oF executions</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT"/>
               </a:p>
@@ -479,7 +1030,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1710589408"/>
+        <c:crossAx val="298922984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -487,7 +1038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1710589408"/>
+        <c:axId val="298922984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -596,7 +1147,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1710590496"/>
+        <c:crossAx val="298921416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -687,10 +1238,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -924,11 +1475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1890209216"/>
-        <c:axId val="-1890196160"/>
+        <c:axId val="298916712"/>
+        <c:axId val="298919064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1890209216"/>
+        <c:axId val="298916712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +1509,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="pt-PT" baseline="0"/>
-                  <a:t> os executions</a:t>
+                  <a:t> oF executions</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT"/>
               </a:p>
@@ -1029,7 +1580,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890196160"/>
+        <c:crossAx val="298919064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1037,7 +1588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1890196160"/>
+        <c:axId val="298919064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1697,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890209216"/>
+        <c:crossAx val="298916712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1237,10 +1788,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1474,11 +2025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1890201056"/>
-        <c:axId val="-1890206496"/>
+        <c:axId val="299114600"/>
+        <c:axId val="299114992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1890201056"/>
+        <c:axId val="299114600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,7 +2130,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890206496"/>
+        <c:crossAx val="299114992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1587,7 +2138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1890206496"/>
+        <c:axId val="299114992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,7 +2242,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890201056"/>
+        <c:crossAx val="299114600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1782,10 +2333,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2062,11 +2613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1890199424"/>
-        <c:axId val="-1890207584"/>
+        <c:axId val="299120872"/>
+        <c:axId val="299114208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1890199424"/>
+        <c:axId val="299120872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2108,7 +2659,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890207584"/>
+        <c:crossAx val="299114208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2116,7 +2667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1890207584"/>
+        <c:axId val="299114208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,7 +2717,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890199424"/>
+        <c:crossAx val="299120872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2180,6 +2731,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2256,10 +2808,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2545,11 +3097,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1890205408"/>
-        <c:axId val="-1890203776"/>
+        <c:axId val="299253856"/>
+        <c:axId val="299255816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1890205408"/>
+        <c:axId val="299253856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +3143,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890203776"/>
+        <c:crossAx val="299255816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2599,7 +3151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1890203776"/>
+        <c:axId val="299255816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,7 +3201,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1890205408"/>
+        <c:crossAx val="299253856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2663,6 +3215,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2939,6 +3492,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -4924,6 +5517,502 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5511,6 +6600,43 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5528,7 +6654,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5565,7 +6691,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5603,7 +6729,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5947,6 +7073,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -5985,7 +7151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -6029,7 +7195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>

</xml_diff>